<commit_message>
finsihed eu sanc index, fixed khi function for >1 rep
</commit_message>
<xml_diff>
--- a/data/comtrade_total_exports_2021A.xlsx
+++ b/data/comtrade_total_exports_2021A.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D150"/>
+  <dimension ref="A1:D162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -445,11 +445,11 @@
         <v>44197</v>
       </c>
       <c r="B5">
-        <v>22207974784.94</v>
+        <v>19147254.49</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Azerbaijan</t>
+          <t>Antigua and Barbuda</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -463,11 +463,11 @@
         <v>44197</v>
       </c>
       <c r="B6">
-        <v>77934314986.58</v>
+        <v>22207974784.94</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Azerbaijan</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -481,11 +481,11 @@
         <v>44197</v>
       </c>
       <c r="B7">
-        <v>342036103269.844</v>
+        <v>77934314986.58</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -499,11 +499,11 @@
         <v>44197</v>
       </c>
       <c r="B8">
-        <v>194703245949.459</v>
+        <v>342036103269.844</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Austria</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -517,11 +517,11 @@
         <v>44197</v>
       </c>
       <c r="B9">
-        <v>18198973799.994</v>
+        <v>194703245949.459</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Bahrain</t>
+          <t>Austria</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -535,11 +535,11 @@
         <v>44197</v>
       </c>
       <c r="B10">
-        <v>2964798290.08</v>
+        <v>18198973799.994</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Armenia</t>
+          <t>Bahrain</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -553,11 +553,11 @@
         <v>44197</v>
       </c>
       <c r="B11">
-        <v>350172911</v>
+        <v>2964798290.08</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Barbados</t>
+          <t>Armenia</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -571,11 +571,11 @@
         <v>44197</v>
       </c>
       <c r="B12">
-        <v>386354055203.238</v>
+        <v>350172911</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Belgium</t>
+          <t>Barbados</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -589,11 +589,11 @@
         <v>44197</v>
       </c>
       <c r="B13">
-        <v>28632529.08</v>
+        <v>385980404667.027</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Bermuda</t>
+          <t>Belgium</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -607,11 +607,11 @@
         <v>44197</v>
       </c>
       <c r="B14">
-        <v>11079788840.24</v>
+        <v>28632529.08</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Bolivia (Plurinational State of)</t>
+          <t>Bermuda</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -625,11 +625,11 @@
         <v>44197</v>
       </c>
       <c r="B15">
-        <v>8614110010.865999</v>
+        <v>11079788840.24</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Bosnia Herzegovina</t>
+          <t>Bolivia (Plurinational State of)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -643,11 +643,11 @@
         <v>44197</v>
       </c>
       <c r="B16">
-        <v>7473466757.015</v>
+        <v>8614110010.865999</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Botswana</t>
+          <t>Bosnia Herzegovina</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -661,11 +661,11 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>280814577460</v>
+        <v>7474891657.999</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Botswana</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -679,11 +679,11 @@
         <v>44197</v>
       </c>
       <c r="B18">
-        <v>264092675.61</v>
+        <v>280814577460</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Belize</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -697,11 +697,11 @@
         <v>44197</v>
       </c>
       <c r="B19">
-        <v>11058184373.01</v>
+        <v>264092675.61</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Brunei Darussalam</t>
+          <t>Belize</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -715,11 +715,11 @@
         <v>44197</v>
       </c>
       <c r="B20">
-        <v>41370856687.293</v>
+        <v>11058184373.01</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Bulgaria</t>
+          <t>Brunei Darussalam</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -733,11 +733,11 @@
         <v>44197</v>
       </c>
       <c r="B21">
-        <v>15144859129.46</v>
+        <v>41370856687.293</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Myanmar</t>
+          <t>Bulgaria</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -751,11 +751,11 @@
         <v>44197</v>
       </c>
       <c r="B22">
-        <v>163656476.675</v>
+        <v>15144859129.46</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Burundi</t>
+          <t>Myanmar</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -769,11 +769,11 @@
         <v>44197</v>
       </c>
       <c r="B23">
-        <v>39889022800</v>
+        <v>163656476.675</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Belarus</t>
+          <t>Burundi</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -787,11 +787,11 @@
         <v>44197</v>
       </c>
       <c r="B24">
-        <v>17571782672.48</v>
+        <v>39889022800</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Cambodia</t>
+          <t>Belarus</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -805,11 +805,11 @@
         <v>44197</v>
       </c>
       <c r="B25">
-        <v>501538854874.334</v>
+        <v>17571782672.48</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>Cambodia</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -823,11 +823,11 @@
         <v>44197</v>
       </c>
       <c r="B26">
-        <v>17082261.232</v>
+        <v>4294055976.357</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Cayman Isds</t>
+          <t>Cameroon</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -841,11 +841,11 @@
         <v>44197</v>
       </c>
       <c r="B27">
-        <v>13331248583.322</v>
+        <v>501538854874.334</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Sri Lanka</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -859,11 +859,11 @@
         <v>44197</v>
       </c>
       <c r="B28">
-        <v>94676809206.28101</v>
+        <v>45366225.058</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>Cabo Verde</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -877,11 +877,11 @@
         <v>44197</v>
       </c>
       <c r="B29">
-        <v>3362301613439</v>
+        <v>17082261.232</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Cayman Isds</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -895,11 +895,11 @@
         <v>44197</v>
       </c>
       <c r="B30">
-        <v>41389989047.59</v>
+        <v>57725502.927</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Central African Rep.</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -913,11 +913,11 @@
         <v>44197</v>
       </c>
       <c r="B31">
-        <v>34994132.52</v>
+        <v>13331248583.322</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Comoros</t>
+          <t>Sri Lanka</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -931,11 +931,11 @@
         <v>44197</v>
       </c>
       <c r="B32">
-        <v>2362230161.01</v>
+        <v>94676809206.28101</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Congo</t>
+          <t>Chile</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -949,11 +949,11 @@
         <v>44197</v>
       </c>
       <c r="B33">
-        <v>24124651297.35</v>
+        <v>3362301613439</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Dem. Rep. of the Congo</t>
+          <t>China</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -967,11 +967,11 @@
         <v>44197</v>
       </c>
       <c r="B34">
-        <v>14345395565.22</v>
+        <v>41389989047.59</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Costa Rica</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -985,11 +985,11 @@
         <v>44197</v>
       </c>
       <c r="B35">
-        <v>21827948964</v>
+        <v>34994132.52</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Croatia</t>
+          <t>Comoros</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1003,11 +1003,11 @@
         <v>44197</v>
       </c>
       <c r="B36">
-        <v>3989812264.347</v>
+        <v>2362230161.01</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Cyprus</t>
+          <t>Congo</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1021,11 +1021,11 @@
         <v>44197</v>
       </c>
       <c r="B37">
-        <v>227168411022</v>
+        <v>24124651297.35</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Czechia</t>
+          <t>Dem. Rep. of the Congo</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1039,11 +1039,11 @@
         <v>44197</v>
       </c>
       <c r="B38">
-        <v>1023522023.899</v>
+        <v>14345395565.22</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Benin</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1057,11 +1057,11 @@
         <v>44197</v>
       </c>
       <c r="B39">
-        <v>125014614347.861</v>
+        <v>21827948964</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Croatia</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1075,11 +1075,11 @@
         <v>44197</v>
       </c>
       <c r="B40">
-        <v>11643220004.19</v>
+        <v>3989812264.347</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Dominican Rep.</t>
+          <t>Cyprus</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1093,11 +1093,11 @@
         <v>44197</v>
       </c>
       <c r="B41">
-        <v>26699199844.372</v>
+        <v>227168411022</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Czechia</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1111,11 +1111,11 @@
         <v>44197</v>
       </c>
       <c r="B42">
-        <v>6394888915.91</v>
+        <v>1023522023.899</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>El Salvador</t>
+          <t>Benin</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1129,11 +1129,11 @@
         <v>44197</v>
       </c>
       <c r="B43">
-        <v>3057628826.59</v>
+        <v>125014614347.861</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Ethiopia</t>
+          <t>Denmark</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1147,11 +1147,11 @@
         <v>44197</v>
       </c>
       <c r="B44">
-        <v>22303230971.07</v>
+        <v>14145191.781</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Estonia</t>
+          <t>Dominica</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1165,11 +1165,11 @@
         <v>44197</v>
       </c>
       <c r="B45">
-        <v>815335653.153</v>
+        <v>11643220004.19</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Fiji</t>
+          <t>Dominican Rep.</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1183,11 +1183,11 @@
         <v>44197</v>
       </c>
       <c r="B46">
-        <v>81500265209.30499</v>
+        <v>26699199844.372</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1201,11 +1201,11 @@
         <v>44197</v>
       </c>
       <c r="B47">
-        <v>585148036598.849</v>
+        <v>6394888915.91</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>El Salvador</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1219,11 +1219,11 @@
         <v>44197</v>
       </c>
       <c r="B48">
-        <v>143139203.697</v>
+        <v>3057628826.59</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>French Polynesia</t>
+          <t>Ethiopia</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1237,11 +1237,11 @@
         <v>44197</v>
       </c>
       <c r="B49">
-        <v>4242512935.07</v>
+        <v>22303230971.07</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Georgia</t>
+          <t>Estonia</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1255,11 +1255,11 @@
         <v>44197</v>
       </c>
       <c r="B50">
-        <v>26401460.44</v>
+        <v>815335653.153</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Gambia</t>
+          <t>Fiji</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1273,11 +1273,11 @@
         <v>44197</v>
       </c>
       <c r="B51">
-        <v>1357640029.17</v>
+        <v>81500265209.30499</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>State of Palestine</t>
+          <t>Finland</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1291,11 +1291,11 @@
         <v>44197</v>
       </c>
       <c r="B52">
-        <v>1635599573787.609</v>
+        <v>585148036598.849</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>France</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1309,11 +1309,11 @@
         <v>44197</v>
       </c>
       <c r="B53">
-        <v>47244277316.697</v>
+        <v>143139203.697</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>French Polynesia</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1327,11 +1327,11 @@
         <v>44197</v>
       </c>
       <c r="B54">
-        <v>35163394.409</v>
+        <v>8031167846.494</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Grenada</t>
+          <t>Gabon</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1345,11 +1345,11 @@
         <v>44197</v>
       </c>
       <c r="B55">
-        <v>13735599195</v>
+        <v>4242512935.07</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Guatemala</t>
+          <t>Georgia</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1363,11 +1363,11 @@
         <v>44197</v>
       </c>
       <c r="B56">
-        <v>4257250461.689</v>
+        <v>26401460.44</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Guyana</t>
+          <t>Gambia</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1381,11 +1381,11 @@
         <v>44197</v>
       </c>
       <c r="B57">
-        <v>4975948988.14</v>
+        <v>1357640029.17</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Honduras</t>
+          <t>State of Palestine</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1399,11 +1399,11 @@
         <v>44197</v>
       </c>
       <c r="B58">
-        <v>670926079457.053</v>
+        <v>1635599573787.609</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>China, Hong Kong SAR</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1417,11 +1417,11 @@
         <v>44197</v>
       </c>
       <c r="B59">
-        <v>141157091681</v>
+        <v>8863588.062000001</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Hungary</t>
+          <t>Kiribati</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1435,11 +1435,11 @@
         <v>44197</v>
       </c>
       <c r="B60">
-        <v>5973742650.46</v>
+        <v>47244277316.697</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Iceland</t>
+          <t>Greece</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1453,11 +1453,11 @@
         <v>44197</v>
       </c>
       <c r="B61">
-        <v>231522458128.8</v>
+        <v>35163394.409</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Indonesia</t>
+          <t>Grenada</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -1471,11 +1471,11 @@
         <v>44197</v>
       </c>
       <c r="B62">
-        <v>195997875900.844</v>
+        <v>13735599195</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Ireland</t>
+          <t>Guatemala</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -1489,11 +1489,11 @@
         <v>44197</v>
       </c>
       <c r="B63">
-        <v>60159734000</v>
+        <v>4257250461.689</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Israel</t>
+          <t>Guyana</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -1507,11 +1507,11 @@
         <v>44197</v>
       </c>
       <c r="B64">
-        <v>615910260060.774</v>
+        <v>4975948988.14</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Honduras</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -1525,11 +1525,11 @@
         <v>44197</v>
       </c>
       <c r="B65">
-        <v>1480709866.69</v>
+        <v>670926079457.053</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Jamaica</t>
+          <t>China, Hong Kong SAR</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -1543,11 +1543,11 @@
         <v>44197</v>
       </c>
       <c r="B66">
-        <v>757066261248.9709</v>
+        <v>141157091681</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Japan</t>
+          <t>Hungary</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -1561,11 +1561,11 @@
         <v>44197</v>
       </c>
       <c r="B67">
-        <v>60321024400.41</v>
+        <v>5973742650.46</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Kazakhstan</t>
+          <t>Iceland</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -1579,11 +1579,11 @@
         <v>44197</v>
       </c>
       <c r="B68">
-        <v>9356550020.493999</v>
+        <v>231522458128.8</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Jordan</t>
+          <t>Indonesia</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -1597,11 +1597,11 @@
         <v>44197</v>
       </c>
       <c r="B69">
-        <v>6751366221.034</v>
+        <v>67271404932.41</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Kenya</t>
+          <t>Iran</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -1615,11 +1615,11 @@
         <v>44197</v>
       </c>
       <c r="B70">
-        <v>644372936752</v>
+        <v>195997875900.844</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Rep. of Korea</t>
+          <t>Ireland</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -1633,11 +1633,11 @@
         <v>44197</v>
       </c>
       <c r="B71">
-        <v>63129693952</v>
+        <v>60159734000</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Kuwait</t>
+          <t>Israel</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -1651,11 +1651,11 @@
         <v>44197</v>
       </c>
       <c r="B72">
-        <v>2752163636</v>
+        <v>615910260060.774</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Kyrgyzstan</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -1669,11 +1669,11 @@
         <v>44197</v>
       </c>
       <c r="B73">
-        <v>7164605459.07</v>
+        <v>15333663013.467</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Lao People's Dem. Rep.</t>
+          <t>Côte d'Ivoire</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -1687,11 +1687,11 @@
         <v>44197</v>
       </c>
       <c r="B74">
-        <v>4229976738</v>
+        <v>1480709866.69</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Lebanon</t>
+          <t>Jamaica</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -1705,11 +1705,11 @@
         <v>44197</v>
       </c>
       <c r="B75">
-        <v>948535188.45</v>
+        <v>757066261248.9709</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Lesotho</t>
+          <t>Japan</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -1723,11 +1723,11 @@
         <v>44197</v>
       </c>
       <c r="B76">
-        <v>19458821916.273</v>
+        <v>60321024400.41</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Latvia</t>
+          <t>Kazakhstan</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -1741,11 +1741,11 @@
         <v>44197</v>
       </c>
       <c r="B77">
-        <v>40698383278.78</v>
+        <v>9356550020.493999</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Lithuania</t>
+          <t>Jordan</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -1759,11 +1759,11 @@
         <v>44197</v>
       </c>
       <c r="B78">
-        <v>16247126542.139</v>
+        <v>6751366221.034</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Luxembourg</t>
+          <t>Kenya</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -1777,11 +1777,11 @@
         <v>44197</v>
       </c>
       <c r="B79">
-        <v>1392424900.553</v>
+        <v>644372936752</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>China, Macao SAR</t>
+          <t>Rep. of Korea</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -1795,11 +1795,11 @@
         <v>44197</v>
       </c>
       <c r="B80">
-        <v>2788376340.521</v>
+        <v>63129693952</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Madagascar</t>
+          <t>Kuwait</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -1813,11 +1813,11 @@
         <v>44197</v>
       </c>
       <c r="B81">
-        <v>1009460778.534</v>
+        <v>2752163636</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Malawi</t>
+          <t>Kyrgyzstan</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -1831,11 +1831,11 @@
         <v>44197</v>
       </c>
       <c r="B82">
-        <v>299230434394.232</v>
+        <v>7164605459.07</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Malaysia</t>
+          <t>Lao People's Dem. Rep.</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -1849,11 +1849,11 @@
         <v>44197</v>
       </c>
       <c r="B83">
-        <v>151293266.49</v>
+        <v>4229976738</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Maldives</t>
+          <t>Lebanon</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -1867,11 +1867,11 @@
         <v>44197</v>
       </c>
       <c r="B84">
-        <v>3066831630.829</v>
+        <v>948535188.45</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Malta</t>
+          <t>Lesotho</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -1885,11 +1885,11 @@
         <v>44197</v>
       </c>
       <c r="B85">
-        <v>3266988807.55</v>
+        <v>19458821916.273</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Mauritania</t>
+          <t>Latvia</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -1903,11 +1903,11 @@
         <v>44197</v>
       </c>
       <c r="B86">
-        <v>1671760288.267</v>
+        <v>40698383278.78</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Mauritius</t>
+          <t>Lithuania</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -1921,11 +1921,11 @@
         <v>44197</v>
       </c>
       <c r="B87">
-        <v>494595503435</v>
+        <v>16247126542.139</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>Luxembourg</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -1939,11 +1939,11 @@
         <v>44197</v>
       </c>
       <c r="B88">
-        <v>447656546120.094</v>
+        <v>1392424900.553</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Other Asia, nes</t>
+          <t>China, Macao SAR</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -1957,11 +1957,11 @@
         <v>44197</v>
       </c>
       <c r="B89">
-        <v>9241123149.940001</v>
+        <v>2788376340.521</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Mongolia</t>
+          <t>Madagascar</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -1975,11 +1975,11 @@
         <v>44197</v>
       </c>
       <c r="B90">
-        <v>3144504817</v>
+        <v>1009460778.534</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Rep. of Moldova</t>
+          <t>Malawi</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -1993,11 +1993,11 @@
         <v>44197</v>
       </c>
       <c r="B91">
-        <v>515916303.811</v>
+        <v>299230434394.232</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Montenegro</t>
+          <t>Malaysia</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -2011,11 +2011,11 @@
         <v>44197</v>
       </c>
       <c r="B92">
-        <v>36585224951.204</v>
+        <v>151293266.49</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Morocco</t>
+          <t>Maldives</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -2029,11 +2029,11 @@
         <v>44197</v>
       </c>
       <c r="B93">
-        <v>5111685900.99</v>
+        <v>3066831630.829</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Mozambique</t>
+          <t>Malta</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -2047,11 +2047,11 @@
         <v>44197</v>
       </c>
       <c r="B94">
-        <v>44590926520.592</v>
+        <v>3266988807.55</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Oman</t>
+          <t>Mauritania</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -2065,11 +2065,11 @@
         <v>44197</v>
       </c>
       <c r="B95">
-        <v>7263807226.853</v>
+        <v>1671760288.267</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Namibia</t>
+          <t>Mauritius</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -2083,11 +2083,11 @@
         <v>44197</v>
       </c>
       <c r="B96">
-        <v>1665727794.55</v>
+        <v>494460765005</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Nepal</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -2101,11 +2101,11 @@
         <v>44197</v>
       </c>
       <c r="B97">
-        <v>696873257184.973</v>
+        <v>447656546120.094</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Netherlands</t>
+          <t>Other Asia, nes</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -2119,11 +2119,11 @@
         <v>44197</v>
       </c>
       <c r="B98">
-        <v>88347007.693</v>
+        <v>9241123149.940001</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Aruba</t>
+          <t>Mongolia</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -2137,11 +2137,11 @@
         <v>44197</v>
       </c>
       <c r="B99">
-        <v>44325287820.466</v>
+        <v>3144504817</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>Rep. of Moldova</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -2155,11 +2155,11 @@
         <v>44197</v>
       </c>
       <c r="B100">
-        <v>6494984866.92</v>
+        <v>515916303.811</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Nicaragua</t>
+          <t>Montenegro</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -2173,11 +2173,11 @@
         <v>44197</v>
       </c>
       <c r="B101">
-        <v>506672560.08</v>
+        <v>36585224951.204</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Niger</t>
+          <t>Morocco</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -2191,11 +2191,11 @@
         <v>44197</v>
       </c>
       <c r="B102">
-        <v>47231712930.364</v>
+        <v>5111685900.99</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Nigeria</t>
+          <t>Mozambique</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -2209,11 +2209,11 @@
         <v>44197</v>
       </c>
       <c r="B103">
-        <v>174513974109.642</v>
+        <v>44590926520.592</v>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Norway</t>
+          <t>Oman</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -2227,11 +2227,11 @@
         <v>44197</v>
       </c>
       <c r="B104">
-        <v>28795179085.962</v>
+        <v>7263807226.853</v>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Pakistan</t>
+          <t>Namibia</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -2245,11 +2245,11 @@
         <v>44197</v>
       </c>
       <c r="B105">
-        <v>3781922651</v>
+        <v>1665727794.55</v>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Panama</t>
+          <t>Nepal</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -2263,11 +2263,11 @@
         <v>44197</v>
       </c>
       <c r="B106">
-        <v>10570969868</v>
+        <v>696873257184.973</v>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Paraguay</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -2281,11 +2281,11 @@
         <v>44197</v>
       </c>
       <c r="B107">
-        <v>56260115202.756</v>
+        <v>88347007.693</v>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Aruba</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -2299,11 +2299,11 @@
         <v>44197</v>
       </c>
       <c r="B108">
-        <v>74619528755</v>
+        <v>44325287820.466</v>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -2317,11 +2317,11 @@
         <v>44197</v>
       </c>
       <c r="B109">
-        <v>317832124942</v>
+        <v>6494984866.92</v>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Poland</t>
+          <t>Nicaragua</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -2335,11 +2335,11 @@
         <v>44197</v>
       </c>
       <c r="B110">
-        <v>75242766894.064</v>
+        <v>506672560.08</v>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Portugal</t>
+          <t>Niger</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -2353,11 +2353,11 @@
         <v>44197</v>
       </c>
       <c r="B111">
-        <v>87203291188.87</v>
+        <v>47231712930.364</v>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Qatar</t>
+          <t>Nigeria</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -2371,11 +2371,11 @@
         <v>44197</v>
       </c>
       <c r="B112">
-        <v>88389728970.91</v>
+        <v>173813766175.705</v>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Romania</t>
+          <t>Norway</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -2389,11 +2389,11 @@
         <v>44197</v>
       </c>
       <c r="B113">
-        <v>492313790696.653</v>
+        <v>28795179085.962</v>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Russian Federation</t>
+          <t>Pakistan</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -2407,11 +2407,11 @@
         <v>44197</v>
       </c>
       <c r="B114">
-        <v>1562504482.7</v>
+        <v>3781922651</v>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Rwanda</t>
+          <t>Panama</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -2425,11 +2425,11 @@
         <v>44197</v>
       </c>
       <c r="B115">
-        <v>34719205.288</v>
+        <v>9650541017.488001</v>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Saint Vincent and the Grenadines</t>
+          <t>Papua New Guinea</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -2443,11 +2443,11 @@
         <v>44197</v>
       </c>
       <c r="B116">
-        <v>19174845.703</v>
+        <v>10570969868</v>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Sao Tome and Principe</t>
+          <t>Paraguay</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -2461,11 +2461,11 @@
         <v>44197</v>
       </c>
       <c r="B117">
-        <v>286467258610.596</v>
+        <v>56260115202.756</v>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Saudi Arabia</t>
+          <t>Peru</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -2479,11 +2479,11 @@
         <v>44197</v>
       </c>
       <c r="B118">
-        <v>5202221589.634</v>
+        <v>74619528755</v>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Senegal</t>
+          <t>Philippines</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -2497,11 +2497,11 @@
         <v>44197</v>
       </c>
       <c r="B119">
-        <v>25566160915</v>
+        <v>317832124942</v>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Serbia</t>
+          <t>Poland</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -2515,11 +2515,11 @@
         <v>44197</v>
       </c>
       <c r="B120">
-        <v>1951925732.167</v>
+        <v>75242766894.064</v>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Seychelles</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -2533,11 +2533,11 @@
         <v>44197</v>
       </c>
       <c r="B121">
-        <v>394813673347.297</v>
+        <v>458303194.55</v>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>Timor-Leste</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -2551,11 +2551,11 @@
         <v>44197</v>
       </c>
       <c r="B122">
-        <v>457081283281.544</v>
+        <v>87203291188.87</v>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Singapore</t>
+          <t>Qatar</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -2569,11 +2569,11 @@
         <v>44197</v>
       </c>
       <c r="B123">
-        <v>104733320881.922</v>
+        <v>88389728970.91</v>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Slovakia</t>
+          <t>Romania</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -2587,11 +2587,11 @@
         <v>44197</v>
       </c>
       <c r="B124">
-        <v>335792597810</v>
+        <v>492313790696.653</v>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Viet Nam</t>
+          <t>Russian Federation</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -2605,11 +2605,11 @@
         <v>44197</v>
       </c>
       <c r="B125">
-        <v>46692128069.11</v>
+        <v>1562504482.7</v>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Slovenia</t>
+          <t>Rwanda</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -2623,11 +2623,11 @@
         <v>44197</v>
       </c>
       <c r="B126">
-        <v>121321278845.567</v>
+        <v>34719205.288</v>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>South Africa</t>
+          <t>Saint Vincent and the Grenadines</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -2641,11 +2641,11 @@
         <v>44197</v>
       </c>
       <c r="B127">
-        <v>6036173160.691</v>
+        <v>19174845.703</v>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Zimbabwe</t>
+          <t>Sao Tome and Principe</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -2659,11 +2659,11 @@
         <v>44197</v>
       </c>
       <c r="B128">
-        <v>391558519476.67</v>
+        <v>286467258610.596</v>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Saudi Arabia</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -2677,11 +2677,11 @@
         <v>44197</v>
       </c>
       <c r="B129">
-        <v>2291325827.04</v>
+        <v>5202221589.634</v>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Suriname</t>
+          <t>Senegal</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -2695,11 +2695,11 @@
         <v>44197</v>
       </c>
       <c r="B130">
-        <v>2068468810.41</v>
+        <v>25566160915</v>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Eswatini</t>
+          <t>Serbia</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -2713,11 +2713,11 @@
         <v>44197</v>
       </c>
       <c r="B131">
-        <v>189635063199.877</v>
+        <v>1951925732.167</v>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Sweden</t>
+          <t>Seychelles</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -2731,11 +2731,11 @@
         <v>44197</v>
       </c>
       <c r="B132">
-        <v>379770927042.891</v>
+        <v>394813673347.297</v>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Switzerland</t>
+          <t>India</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
@@ -2749,11 +2749,11 @@
         <v>44197</v>
       </c>
       <c r="B133">
-        <v>1476799996</v>
+        <v>457081283281.544</v>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>Tajikistan</t>
+          <t>Singapore</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -2767,11 +2767,11 @@
         <v>44197</v>
       </c>
       <c r="B134">
-        <v>266674796256.73</v>
+        <v>104733320881.922</v>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>Slovakia</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -2785,11 +2785,11 @@
         <v>44197</v>
       </c>
       <c r="B135">
-        <v>1079792672.912</v>
+        <v>335792597810</v>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Togo</t>
+          <t>Viet Nam</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -2803,11 +2803,11 @@
         <v>44197</v>
       </c>
       <c r="B136">
-        <v>8620228624.916</v>
+        <v>46692128069.11</v>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>Trinidad and Tobago</t>
+          <t>Slovenia</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -2821,11 +2821,11 @@
         <v>44197</v>
       </c>
       <c r="B137">
-        <v>425159796503.562</v>
+        <v>121321278845.567</v>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>United Arab Emirates</t>
+          <t>South Africa</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -2839,11 +2839,11 @@
         <v>44197</v>
       </c>
       <c r="B138">
-        <v>16695198641.544</v>
+        <v>6036173160.691</v>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Tunisia</t>
+          <t>Zimbabwe</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -2857,11 +2857,11 @@
         <v>44197</v>
       </c>
       <c r="B139">
-        <v>225214458038</v>
+        <v>391558519476.67</v>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Türkiye</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -2875,11 +2875,11 @@
         <v>44197</v>
       </c>
       <c r="B140">
-        <v>65870275510.39</v>
+        <v>2291325827.04</v>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Ukraine</t>
+          <t>Suriname</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
@@ -2893,11 +2893,11 @@
         <v>44197</v>
       </c>
       <c r="B141">
-        <v>8186314637.628</v>
+        <v>2068468810.41</v>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>North Macedonia</t>
+          <t>Eswatini</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
@@ -2911,11 +2911,11 @@
         <v>44197</v>
       </c>
       <c r="B142">
-        <v>40701703944.38</v>
+        <v>189635063199.877</v>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Egypt</t>
+          <t>Sweden</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
@@ -2929,11 +2929,11 @@
         <v>44197</v>
       </c>
       <c r="B143">
-        <v>470547786029.463</v>
+        <v>379770927042.891</v>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>United Kingdom</t>
+          <t>Switzerland</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
@@ -2947,11 +2947,11 @@
         <v>44197</v>
       </c>
       <c r="B144">
-        <v>6390862886.744</v>
+        <v>1476799996</v>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>United Rep. of Tanzania</t>
+          <t>Tajikistan</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -2965,11 +2965,11 @@
         <v>44197</v>
       </c>
       <c r="B145">
-        <v>1753136708106</v>
+        <v>266674796256.73</v>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>Thailand</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
@@ -2983,11 +2983,11 @@
         <v>44197</v>
       </c>
       <c r="B146">
-        <v>5060027958.95</v>
+        <v>1079792672.912</v>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>Burkina Faso</t>
+          <t>Togo</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
@@ -3001,11 +3001,11 @@
         <v>44197</v>
       </c>
       <c r="B147">
-        <v>9541020289</v>
+        <v>8620228624.916</v>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>Uruguay</t>
+          <t>Trinidad and Tobago</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
@@ -3019,11 +3019,11 @@
         <v>44197</v>
       </c>
       <c r="B148">
-        <v>14092247992.431</v>
+        <v>425159796503.562</v>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>Uzbekistan</t>
+          <t>United Arab Emirates</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -3037,11 +3037,11 @@
         <v>44197</v>
       </c>
       <c r="B149">
-        <v>28836585.461</v>
+        <v>16695198641.544</v>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>Samoa</t>
+          <t>Tunisia</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
@@ -3055,14 +3055,230 @@
         <v>44197</v>
       </c>
       <c r="B150">
+        <v>225214458038</v>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>Türkiye</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>World</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B151">
+        <v>3965317044.55</v>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>Uganda</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>World</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B152">
+        <v>65870275510.39</v>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>Ukraine</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>World</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B153">
+        <v>8186314637.628</v>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>North Macedonia</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>World</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B154">
+        <v>40701703944.38</v>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>Egypt</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>World</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B155">
+        <v>470547786029.463</v>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>United Kingdom</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>World</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B156">
+        <v>6390862886.744</v>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>United Rep. of Tanzania</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>World</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B157">
+        <v>1753136708106</v>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>World</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B158">
+        <v>5060027958.95</v>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>Burkina Faso</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>World</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B159">
+        <v>9541020289</v>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>Uruguay</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>World</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B160">
+        <v>14092247992.431</v>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>Uzbekistan</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>World</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B161">
+        <v>28836585.461</v>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>Samoa</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>World</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B162">
         <v>10101351858.32</v>
       </c>
-      <c r="C150" t="inlineStr">
+      <c r="C162" t="inlineStr">
         <is>
           <t>Zambia</t>
         </is>
       </c>
-      <c r="D150" t="inlineStr">
+      <c r="D162" t="inlineStr">
         <is>
           <t>World</t>
         </is>

</xml_diff>

<commit_message>
updated api key setter
</commit_message>
<xml_diff>
--- a/data/comtrade_total_exports_2021A.xlsx
+++ b/data/comtrade_total_exports_2021A.xlsx
@@ -949,7 +949,7 @@
         <v>44197</v>
       </c>
       <c r="B33">
-        <v>3362301613439</v>
+        <v>3316022133985</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -985,7 +985,7 @@
         <v>44197</v>
       </c>
       <c r="B35">
-        <v>34994132.52</v>
+        <v>34222278.682</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1021,7 +1021,7 @@
         <v>44197</v>
       </c>
       <c r="B37">
-        <v>24124651297.35</v>
+        <v>21412416606.361</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1291,7 +1291,7 @@
         <v>44197</v>
       </c>
       <c r="B52">
-        <v>585148036598.849</v>
+        <v>585395916302.973</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1957,7 +1957,7 @@
         <v>44197</v>
       </c>
       <c r="B89">
-        <v>2788376340.521</v>
+        <v>2788495475.762</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -2047,7 +2047,7 @@
         <v>44197</v>
       </c>
       <c r="B94">
-        <v>3266988807.55</v>
+        <v>3266988807.77</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -2191,7 +2191,7 @@
         <v>44197</v>
       </c>
       <c r="B102">
-        <v>5111685900.99</v>
+        <v>5704483311.693</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
@@ -2227,7 +2227,7 @@
         <v>44197</v>
       </c>
       <c r="B104">
-        <v>7263807226.853</v>
+        <v>4417050677.857</v>
       </c>
       <c r="C104" t="inlineStr">
         <is>
@@ -2335,7 +2335,7 @@
         <v>44197</v>
       </c>
       <c r="B110">
-        <v>506672560.08</v>
+        <v>737116422.265</v>
       </c>
       <c r="C110" t="inlineStr">
         <is>
@@ -2713,7 +2713,7 @@
         <v>44197</v>
       </c>
       <c r="B131">
-        <v>1951925732.167</v>
+        <v>633870713.4859999</v>
       </c>
       <c r="C131" t="inlineStr">
         <is>
@@ -2839,7 +2839,7 @@
         <v>44197</v>
       </c>
       <c r="B138">
-        <v>6036173160.691</v>
+        <v>6036188264.211</v>
       </c>
       <c r="C138" t="inlineStr">
         <is>
@@ -3217,7 +3217,7 @@
         <v>44197</v>
       </c>
       <c r="B159">
-        <v>9541020289</v>
+        <v>9535273938</v>
       </c>
       <c r="C159" t="inlineStr">
         <is>
@@ -3271,7 +3271,7 @@
         <v>44197</v>
       </c>
       <c r="B162">
-        <v>10101351858.32</v>
+        <v>11013140616.688</v>
       </c>
       <c r="C162" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
changed date seq code
</commit_message>
<xml_diff>
--- a/data/comtrade_total_exports_2021A.xlsx
+++ b/data/comtrade_total_exports_2021A.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D162"/>
+  <dimension ref="A1:D163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1417,11 +1417,11 @@
         <v>44197</v>
       </c>
       <c r="B59">
-        <v>8863588.062000001</v>
+        <v>14823232488.086</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Kiribati</t>
+          <t>Ghana</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1435,11 +1435,11 @@
         <v>44197</v>
       </c>
       <c r="B60">
-        <v>47244277316.697</v>
+        <v>8863588.062000001</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>Kiribati</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1453,11 +1453,11 @@
         <v>44197</v>
       </c>
       <c r="B61">
-        <v>35163394.409</v>
+        <v>47244277316.697</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Grenada</t>
+          <t>Greece</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -1471,11 +1471,11 @@
         <v>44197</v>
       </c>
       <c r="B62">
-        <v>13735599195</v>
+        <v>35163394.409</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Guatemala</t>
+          <t>Grenada</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -1489,11 +1489,11 @@
         <v>44197</v>
       </c>
       <c r="B63">
-        <v>8707906391.507999</v>
+        <v>13735599195</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Guyana</t>
+          <t>Guatemala</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -1507,11 +1507,11 @@
         <v>44197</v>
       </c>
       <c r="B64">
-        <v>4975948988.14</v>
+        <v>8707906391.507999</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Honduras</t>
+          <t>Guyana</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -1525,11 +1525,11 @@
         <v>44197</v>
       </c>
       <c r="B65">
-        <v>670926079457.053</v>
+        <v>4975948988.14</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>China, Hong Kong SAR</t>
+          <t>Honduras</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -1543,11 +1543,11 @@
         <v>44197</v>
       </c>
       <c r="B66">
-        <v>141157091681</v>
+        <v>670926079457.053</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Hungary</t>
+          <t>China, Hong Kong SAR</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -1561,11 +1561,11 @@
         <v>44197</v>
       </c>
       <c r="B67">
-        <v>5973742650.46</v>
+        <v>141157091681</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Iceland</t>
+          <t>Hungary</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -1579,11 +1579,11 @@
         <v>44197</v>
       </c>
       <c r="B68">
-        <v>231522458128.8</v>
+        <v>5973742650.46</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Indonesia</t>
+          <t>Iceland</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -1597,11 +1597,11 @@
         <v>44197</v>
       </c>
       <c r="B69">
-        <v>67271404932.41</v>
+        <v>231522458128.8</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Iran</t>
+          <t>Indonesia</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -1615,11 +1615,11 @@
         <v>44197</v>
       </c>
       <c r="B70">
-        <v>195997875885.468</v>
+        <v>67271404932.41</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Ireland</t>
+          <t>Iran</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -1633,11 +1633,11 @@
         <v>44197</v>
       </c>
       <c r="B71">
-        <v>60159734000</v>
+        <v>195997875885.468</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Israel</t>
+          <t>Ireland</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -1651,11 +1651,11 @@
         <v>44197</v>
       </c>
       <c r="B72">
-        <v>615910260060.774</v>
+        <v>60159734000</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Israel</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -1669,11 +1669,11 @@
         <v>44197</v>
       </c>
       <c r="B73">
-        <v>15333663013.467</v>
+        <v>615910260060.774</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Côte d'Ivoire</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -1687,11 +1687,11 @@
         <v>44197</v>
       </c>
       <c r="B74">
-        <v>1480709866.69</v>
+        <v>15333663013.467</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Jamaica</t>
+          <t>Côte d'Ivoire</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -1705,11 +1705,11 @@
         <v>44197</v>
       </c>
       <c r="B75">
-        <v>757066261248.9709</v>
+        <v>1480709866.69</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Japan</t>
+          <t>Jamaica</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -1723,11 +1723,11 @@
         <v>44197</v>
       </c>
       <c r="B76">
-        <v>60321024400.41</v>
+        <v>757066261248.9709</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Kazakhstan</t>
+          <t>Japan</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -1741,11 +1741,11 @@
         <v>44197</v>
       </c>
       <c r="B77">
-        <v>9356550020.493999</v>
+        <v>60321024400.41</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Jordan</t>
+          <t>Kazakhstan</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -1759,11 +1759,11 @@
         <v>44197</v>
       </c>
       <c r="B78">
-        <v>6751366221.034</v>
+        <v>9356550020.493999</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Kenya</t>
+          <t>Jordan</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -1777,11 +1777,11 @@
         <v>44197</v>
       </c>
       <c r="B79">
-        <v>644372936752</v>
+        <v>6751366221.034</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Rep. of Korea</t>
+          <t>Kenya</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -1795,11 +1795,11 @@
         <v>44197</v>
       </c>
       <c r="B80">
-        <v>63129693952</v>
+        <v>644372936752</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Kuwait</t>
+          <t>Rep. of Korea</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -1813,11 +1813,11 @@
         <v>44197</v>
       </c>
       <c r="B81">
-        <v>2752163636</v>
+        <v>63129693952</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Kyrgyzstan</t>
+          <t>Kuwait</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -1831,11 +1831,11 @@
         <v>44197</v>
       </c>
       <c r="B82">
-        <v>7164605459.07</v>
+        <v>2752163636</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Lao People's Dem. Rep.</t>
+          <t>Kyrgyzstan</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -1849,11 +1849,11 @@
         <v>44197</v>
       </c>
       <c r="B83">
-        <v>4229976738</v>
+        <v>7164605459.07</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Lebanon</t>
+          <t>Lao People's Dem. Rep.</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -1867,11 +1867,11 @@
         <v>44197</v>
       </c>
       <c r="B84">
-        <v>948535188.45</v>
+        <v>4229976738</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Lesotho</t>
+          <t>Lebanon</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -1885,11 +1885,11 @@
         <v>44197</v>
       </c>
       <c r="B85">
-        <v>19458821916.273</v>
+        <v>948535188.45</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Latvia</t>
+          <t>Lesotho</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -1903,11 +1903,11 @@
         <v>44197</v>
       </c>
       <c r="B86">
-        <v>40698383278.78</v>
+        <v>19458821916.273</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Lithuania</t>
+          <t>Latvia</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -1921,11 +1921,11 @@
         <v>44197</v>
       </c>
       <c r="B87">
-        <v>16247126542.139</v>
+        <v>40698383278.78</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Luxembourg</t>
+          <t>Lithuania</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -1939,11 +1939,11 @@
         <v>44197</v>
       </c>
       <c r="B88">
-        <v>1392424900.553</v>
+        <v>16247126542.139</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>China, Macao SAR</t>
+          <t>Luxembourg</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -1957,11 +1957,11 @@
         <v>44197</v>
       </c>
       <c r="B89">
-        <v>2788495475.762</v>
+        <v>1392424900.553</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Madagascar</t>
+          <t>China, Macao SAR</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -1975,11 +1975,11 @@
         <v>44197</v>
       </c>
       <c r="B90">
-        <v>1009460778.534</v>
+        <v>2788495475.762</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Malawi</t>
+          <t>Madagascar</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -1993,11 +1993,11 @@
         <v>44197</v>
       </c>
       <c r="B91">
-        <v>299230434394.232</v>
+        <v>1009460778.534</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Malaysia</t>
+          <t>Malawi</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -2011,11 +2011,11 @@
         <v>44197</v>
       </c>
       <c r="B92">
-        <v>151293266.49</v>
+        <v>299230434394.232</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Maldives</t>
+          <t>Malaysia</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -2029,11 +2029,11 @@
         <v>44197</v>
       </c>
       <c r="B93">
-        <v>3066831630.829</v>
+        <v>151293266.49</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Malta</t>
+          <t>Maldives</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -2047,11 +2047,11 @@
         <v>44197</v>
       </c>
       <c r="B94">
-        <v>3266988807.77</v>
+        <v>3066831630.829</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Mauritania</t>
+          <t>Malta</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -2065,11 +2065,11 @@
         <v>44197</v>
       </c>
       <c r="B95">
-        <v>1671760288.267</v>
+        <v>3266988807.77</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Mauritius</t>
+          <t>Mauritania</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -2083,11 +2083,11 @@
         <v>44197</v>
       </c>
       <c r="B96">
-        <v>494460765005</v>
+        <v>1671760288.267</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>Mauritius</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -2101,11 +2101,11 @@
         <v>44197</v>
       </c>
       <c r="B97">
-        <v>447656546120.094</v>
+        <v>494460765005</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Other Asia, nes</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -2119,11 +2119,11 @@
         <v>44197</v>
       </c>
       <c r="B98">
-        <v>9241123149.940001</v>
+        <v>447656546120.094</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Mongolia</t>
+          <t>Other Asia, nes</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -2137,11 +2137,11 @@
         <v>44197</v>
       </c>
       <c r="B99">
-        <v>3144504817</v>
+        <v>9241123149.940001</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Rep. of Moldova</t>
+          <t>Mongolia</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -2155,11 +2155,11 @@
         <v>44197</v>
       </c>
       <c r="B100">
-        <v>515916303.811</v>
+        <v>3144504817</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Montenegro</t>
+          <t>Rep. of Moldova</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -2173,11 +2173,11 @@
         <v>44197</v>
       </c>
       <c r="B101">
-        <v>36585224951.204</v>
+        <v>515916303.811</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Morocco</t>
+          <t>Montenegro</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -2191,11 +2191,11 @@
         <v>44197</v>
       </c>
       <c r="B102">
-        <v>5704483311.693</v>
+        <v>36585224951.204</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Mozambique</t>
+          <t>Morocco</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -2209,11 +2209,11 @@
         <v>44197</v>
       </c>
       <c r="B103">
-        <v>44590926520.592</v>
+        <v>5704483311.693</v>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Oman</t>
+          <t>Mozambique</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -2227,11 +2227,11 @@
         <v>44197</v>
       </c>
       <c r="B104">
-        <v>4417050677.857</v>
+        <v>44590926520.592</v>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Namibia</t>
+          <t>Oman</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -2245,11 +2245,11 @@
         <v>44197</v>
       </c>
       <c r="B105">
-        <v>1665727794.55</v>
+        <v>4417050677.857</v>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Nepal</t>
+          <t>Namibia</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -2263,11 +2263,11 @@
         <v>44197</v>
       </c>
       <c r="B106">
-        <v>696873257184.973</v>
+        <v>1665727794.55</v>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Netherlands</t>
+          <t>Nepal</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -2281,11 +2281,11 @@
         <v>44197</v>
       </c>
       <c r="B107">
-        <v>88347007.693</v>
+        <v>696873257184.973</v>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Aruba</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -2299,11 +2299,11 @@
         <v>44197</v>
       </c>
       <c r="B108">
-        <v>44325287820.466</v>
+        <v>88347007.693</v>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>Aruba</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -2317,11 +2317,11 @@
         <v>44197</v>
       </c>
       <c r="B109">
-        <v>6494984866.92</v>
+        <v>44325287820.466</v>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Nicaragua</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -2335,11 +2335,11 @@
         <v>44197</v>
       </c>
       <c r="B110">
-        <v>737116422.265</v>
+        <v>6494984866.92</v>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Niger</t>
+          <t>Nicaragua</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -2353,11 +2353,11 @@
         <v>44197</v>
       </c>
       <c r="B111">
-        <v>47231712930.364</v>
+        <v>737116422.265</v>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Nigeria</t>
+          <t>Niger</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -2371,11 +2371,11 @@
         <v>44197</v>
       </c>
       <c r="B112">
-        <v>173813766175.705</v>
+        <v>47231712930.364</v>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Norway</t>
+          <t>Nigeria</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -2389,11 +2389,11 @@
         <v>44197</v>
       </c>
       <c r="B113">
-        <v>28795179085.962</v>
+        <v>173813766175.705</v>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Pakistan</t>
+          <t>Norway</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -2407,11 +2407,11 @@
         <v>44197</v>
       </c>
       <c r="B114">
-        <v>3781922651</v>
+        <v>28795179085.962</v>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Panama</t>
+          <t>Pakistan</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -2425,11 +2425,11 @@
         <v>44197</v>
       </c>
       <c r="B115">
-        <v>9650541017.488001</v>
+        <v>3781922651</v>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Papua New Guinea</t>
+          <t>Panama</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -2443,11 +2443,11 @@
         <v>44197</v>
       </c>
       <c r="B116">
-        <v>10570969868</v>
+        <v>9650541017.488001</v>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Paraguay</t>
+          <t>Papua New Guinea</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -2461,11 +2461,11 @@
         <v>44197</v>
       </c>
       <c r="B117">
-        <v>56260115202.756</v>
+        <v>10570969868</v>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Paraguay</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -2479,11 +2479,11 @@
         <v>44197</v>
       </c>
       <c r="B118">
-        <v>74619528755</v>
+        <v>56260115202.756</v>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Peru</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -2497,11 +2497,11 @@
         <v>44197</v>
       </c>
       <c r="B119">
-        <v>317832124942</v>
+        <v>74619528755</v>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Poland</t>
+          <t>Philippines</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -2515,11 +2515,11 @@
         <v>44197</v>
       </c>
       <c r="B120">
-        <v>75242766894.064</v>
+        <v>317832124942</v>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Portugal</t>
+          <t>Poland</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -2533,11 +2533,11 @@
         <v>44197</v>
       </c>
       <c r="B121">
-        <v>458303194.55</v>
+        <v>75242766894.064</v>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Timor-Leste</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -2551,11 +2551,11 @@
         <v>44197</v>
       </c>
       <c r="B122">
-        <v>87203291188.87</v>
+        <v>458303194.55</v>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Qatar</t>
+          <t>Timor-Leste</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -2569,11 +2569,11 @@
         <v>44197</v>
       </c>
       <c r="B123">
-        <v>88389728970.91</v>
+        <v>87203291188.87</v>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Romania</t>
+          <t>Qatar</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -2587,11 +2587,11 @@
         <v>44197</v>
       </c>
       <c r="B124">
-        <v>492313790696.653</v>
+        <v>88389728970.91</v>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Russian Federation</t>
+          <t>Romania</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -2605,11 +2605,11 @@
         <v>44197</v>
       </c>
       <c r="B125">
-        <v>1562504482.7</v>
+        <v>492313790696.653</v>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Rwanda</t>
+          <t>Russian Federation</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -2623,11 +2623,11 @@
         <v>44197</v>
       </c>
       <c r="B126">
-        <v>34719205.288</v>
+        <v>1562504482.7</v>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Saint Vincent and the Grenadines</t>
+          <t>Rwanda</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -2641,11 +2641,11 @@
         <v>44197</v>
       </c>
       <c r="B127">
-        <v>19174845.703</v>
+        <v>34719205.288</v>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Sao Tome and Principe</t>
+          <t>Saint Vincent and the Grenadines</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -2659,11 +2659,11 @@
         <v>44197</v>
       </c>
       <c r="B128">
-        <v>286467258610.596</v>
+        <v>19174845.703</v>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Saudi Arabia</t>
+          <t>Sao Tome and Principe</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -2677,11 +2677,11 @@
         <v>44197</v>
       </c>
       <c r="B129">
-        <v>5202221589.634</v>
+        <v>286467258610.596</v>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Senegal</t>
+          <t>Saudi Arabia</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -2695,11 +2695,11 @@
         <v>44197</v>
       </c>
       <c r="B130">
-        <v>25566160915</v>
+        <v>5202221589.634</v>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Serbia</t>
+          <t>Senegal</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -2713,11 +2713,11 @@
         <v>44197</v>
       </c>
       <c r="B131">
-        <v>633870713.4859999</v>
+        <v>25566160915</v>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Seychelles</t>
+          <t>Serbia</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -2731,11 +2731,11 @@
         <v>44197</v>
       </c>
       <c r="B132">
-        <v>394813673347.297</v>
+        <v>633870713.4859999</v>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>Seychelles</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
@@ -2749,11 +2749,11 @@
         <v>44197</v>
       </c>
       <c r="B133">
-        <v>457081283281.544</v>
+        <v>394813673347.297</v>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>Singapore</t>
+          <t>India</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -2767,11 +2767,11 @@
         <v>44197</v>
       </c>
       <c r="B134">
-        <v>104733320881.922</v>
+        <v>457081283281.544</v>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Slovakia</t>
+          <t>Singapore</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -2785,11 +2785,11 @@
         <v>44197</v>
       </c>
       <c r="B135">
-        <v>335792597810</v>
+        <v>104733320881.922</v>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Viet Nam</t>
+          <t>Slovakia</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -2803,11 +2803,11 @@
         <v>44197</v>
       </c>
       <c r="B136">
-        <v>46692128069.11</v>
+        <v>335792597810</v>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>Slovenia</t>
+          <t>Viet Nam</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -2821,11 +2821,11 @@
         <v>44197</v>
       </c>
       <c r="B137">
-        <v>121321278845.567</v>
+        <v>46692128069.11</v>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>South Africa</t>
+          <t>Slovenia</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -2839,11 +2839,11 @@
         <v>44197</v>
       </c>
       <c r="B138">
-        <v>6036188240.041</v>
+        <v>121321278845.567</v>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Zimbabwe</t>
+          <t>South Africa</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -2857,11 +2857,11 @@
         <v>44197</v>
       </c>
       <c r="B139">
-        <v>391558519476.67</v>
+        <v>6036188240.041</v>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Zimbabwe</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -2875,11 +2875,11 @@
         <v>44197</v>
       </c>
       <c r="B140">
-        <v>2291325827.04</v>
+        <v>391558519476.67</v>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Suriname</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
@@ -2893,11 +2893,11 @@
         <v>44197</v>
       </c>
       <c r="B141">
-        <v>2068468810.41</v>
+        <v>2291325827.04</v>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Eswatini</t>
+          <t>Suriname</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
@@ -2911,11 +2911,11 @@
         <v>44197</v>
       </c>
       <c r="B142">
-        <v>189635063199.877</v>
+        <v>2068468810.41</v>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Sweden</t>
+          <t>Eswatini</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
@@ -2929,11 +2929,11 @@
         <v>44197</v>
       </c>
       <c r="B143">
-        <v>379770927042.891</v>
+        <v>189635063199.877</v>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Switzerland</t>
+          <t>Sweden</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
@@ -2947,11 +2947,11 @@
         <v>44197</v>
       </c>
       <c r="B144">
-        <v>1476799996</v>
+        <v>379770927042.891</v>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>Tajikistan</t>
+          <t>Switzerland</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -2965,11 +2965,11 @@
         <v>44197</v>
       </c>
       <c r="B145">
-        <v>266674796256.73</v>
+        <v>1476799996</v>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>Tajikistan</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
@@ -2983,11 +2983,11 @@
         <v>44197</v>
       </c>
       <c r="B146">
-        <v>1059661549.336</v>
+        <v>266674796256.73</v>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>Togo</t>
+          <t>Thailand</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
@@ -3001,11 +3001,11 @@
         <v>44197</v>
       </c>
       <c r="B147">
-        <v>8620228624.916</v>
+        <v>1059661549.336</v>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>Trinidad and Tobago</t>
+          <t>Togo</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
@@ -3019,11 +3019,11 @@
         <v>44197</v>
       </c>
       <c r="B148">
-        <v>425159796503.562</v>
+        <v>8620228624.916</v>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>United Arab Emirates</t>
+          <t>Trinidad and Tobago</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -3037,11 +3037,11 @@
         <v>44197</v>
       </c>
       <c r="B149">
-        <v>16695198641.544</v>
+        <v>425159796503.562</v>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>Tunisia</t>
+          <t>United Arab Emirates</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
@@ -3055,11 +3055,11 @@
         <v>44197</v>
       </c>
       <c r="B150">
-        <v>225214458038</v>
+        <v>16695198641.544</v>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>Türkiye</t>
+          <t>Tunisia</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
@@ -3073,11 +3073,11 @@
         <v>44197</v>
       </c>
       <c r="B151">
-        <v>3965317044.55</v>
+        <v>225214458038</v>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>Uganda</t>
+          <t>Türkiye</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
@@ -3091,11 +3091,11 @@
         <v>44197</v>
       </c>
       <c r="B152">
-        <v>65870275510.39</v>
+        <v>3965317044.55</v>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>Ukraine</t>
+          <t>Uganda</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
@@ -3109,11 +3109,11 @@
         <v>44197</v>
       </c>
       <c r="B153">
-        <v>8186314637.628</v>
+        <v>65870275510.39</v>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>North Macedonia</t>
+          <t>Ukraine</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
@@ -3127,11 +3127,11 @@
         <v>44197</v>
       </c>
       <c r="B154">
-        <v>40701703944.38</v>
+        <v>8186314637.628</v>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>Egypt</t>
+          <t>North Macedonia</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
@@ -3145,11 +3145,11 @@
         <v>44197</v>
       </c>
       <c r="B155">
-        <v>470547786029.463</v>
+        <v>40701703944.38</v>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>United Kingdom</t>
+          <t>Egypt</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
@@ -3163,11 +3163,11 @@
         <v>44197</v>
       </c>
       <c r="B156">
-        <v>6390862886.744</v>
+        <v>470547786029.463</v>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>United Rep. of Tanzania</t>
+          <t>United Kingdom</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
@@ -3181,11 +3181,11 @@
         <v>44197</v>
       </c>
       <c r="B157">
-        <v>1753136708106</v>
+        <v>6390862886.744</v>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>United Rep. of Tanzania</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
@@ -3199,11 +3199,11 @@
         <v>44197</v>
       </c>
       <c r="B158">
-        <v>5060027958.95</v>
+        <v>1753136708106</v>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>Burkina Faso</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
@@ -3217,11 +3217,11 @@
         <v>44197</v>
       </c>
       <c r="B159">
-        <v>9535273938</v>
+        <v>5060027958.95</v>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>Uruguay</t>
+          <t>Burkina Faso</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
@@ -3235,11 +3235,11 @@
         <v>44197</v>
       </c>
       <c r="B160">
-        <v>14092247992.431</v>
+        <v>9535273938</v>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>Uzbekistan</t>
+          <t>Uruguay</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
@@ -3253,11 +3253,11 @@
         <v>44197</v>
       </c>
       <c r="B161">
-        <v>28836585.461</v>
+        <v>14092247992.431</v>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>Samoa</t>
+          <t>Uzbekistan</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
@@ -3271,14 +3271,32 @@
         <v>44197</v>
       </c>
       <c r="B162">
+        <v>28836585.461</v>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>Samoa</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>World</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B163">
         <v>11013140616.688</v>
       </c>
-      <c r="C162" t="inlineStr">
+      <c r="C163" t="inlineStr">
         <is>
           <t>Zambia</t>
         </is>
       </c>
-      <c r="D162" t="inlineStr">
+      <c r="D163" t="inlineStr">
         <is>
           <t>World</t>
         </is>

</xml_diff>